<commit_message>
reformated the code and added functionality
</commit_message>
<xml_diff>
--- a/MET values.xlsx
+++ b/MET values.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Activity</t>
   </si>
@@ -66,6 +66,9 @@
   </si>
   <si>
     <t>snow shoveling</t>
+  </si>
+  <si>
+    <t>Running</t>
   </si>
 </sst>
 </file>
@@ -383,14 +386,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E27"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="43" customWidth="1"/>
     <col min="2" max="2" width="19.28515625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -428,7 +432,7 @@
         <v>13</v>
       </c>
       <c r="C3">
-        <f t="shared" ref="C3:C27" si="0">200/1/109*B3</f>
+        <f t="shared" ref="C3:C12" si="0">200/1/109*B3</f>
         <v>23.853211009174313</v>
       </c>
     </row>
@@ -529,99 +533,15 @@
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12">
+        <v>22</v>
+      </c>
       <c r="C12">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C13">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C14">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C15">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C17">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C18">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C19">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C20">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C21">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C22">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C23">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C24">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C25">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C26">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C27">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>40.366972477064223</v>
       </c>
     </row>
   </sheetData>

</xml_diff>